<commit_message>
añade tablas a la sección 02
</commit_message>
<xml_diff>
--- a/Índice de Tablas (16-01-2017).xlsx
+++ b/Índice de Tablas (16-01-2017).xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe Mc\Dropbox\Observatorio Laboral\Web OLN\Documentos entregados a Austranet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Documents\GitHub\OLN-ISN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -69,12 +69,12 @@
     <definedName name="_ftn1" localSheetId="5">'1.4'!#REF!</definedName>
     <definedName name="_ftnref1" localSheetId="5">'1.4'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="427">
   <si>
     <t>Tramo de edad</t>
   </si>
@@ -1401,25 +1401,35 @@
   <si>
     <t>5.11. Características generales de las principales ocupaciones ejercidas en el sector Administración Pública, 2015</t>
   </si>
+  <si>
+    <t>Esta Tabla es idéntica a la Tabla 5.3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="8">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="170" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="54" x14ac:knownFonts="1">
+  <fonts count="55" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2128,807 +2138,807 @@
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="24"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24"/>
+    <xf numFmtId="43" fontId="40" fillId="0" borderId="24" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="24"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24"/>
-    <xf numFmtId="167" fontId="39" fillId="0" borderId="24" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="24" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="24" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="24" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="24" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="399">
+  <cellXfs count="400">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="20" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="21" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="24" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="28" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="30" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="31" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="31" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="32" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="11" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="15" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="25" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="14" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="25" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="21" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="41" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="41" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="25" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="41" fillId="2" borderId="25" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="41" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="25" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="41" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="41" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="41" fillId="2" borderId="25" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="41" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="21" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="2" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="41" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="41" fillId="0" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="41" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="25" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="21" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="24" xfId="9" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="24" xfId="9" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="9" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="24" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="42" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="42" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="25" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="42" fillId="2" borderId="25" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="42" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="25" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="42" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="42" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="42" fillId="2" borderId="25" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="42" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="21" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="42" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="42" fillId="0" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="42" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="25" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="24" xfId="9" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="24" xfId="9" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="9" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="24" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="30" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="30" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="30" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="30" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="30" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="30" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="24" xfId="9" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="24" xfId="9" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="2" borderId="24" xfId="9" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="24" xfId="9" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="2" borderId="1" xfId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="1" xfId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="18" fillId="2" borderId="24" xfId="10" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="18" fillId="2" borderId="24" xfId="9" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="18" fillId="2" borderId="24" xfId="9" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="2" borderId="24" xfId="10" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="19" fillId="2" borderId="24" xfId="9" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="19" fillId="2" borderId="24" xfId="9" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="42" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="42" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="2" borderId="25" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="42" fillId="2" borderId="25" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="8" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="8" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="8" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="8" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="8" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="8" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="8" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="8" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="24" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="8" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="24" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="8" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="25" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="25" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="25" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="25" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="3" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="3" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="3" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="8" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="54" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="8"/>
-    <xf numFmtId="164" fontId="41" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="41" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="41" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="8"/>
+    <xf numFmtId="165" fontId="42" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="42" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="42" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="42" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="25" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="25" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="2" borderId="24" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="11" fillId="2" borderId="24" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="2" borderId="25" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="11" fillId="2" borderId="25" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="2" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="2" borderId="24" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="2" borderId="24" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="2" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="2" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="2" borderId="25" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="2" borderId="25" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="24" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="3" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="41" fillId="2" borderId="24" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="42" fillId="2" borderId="24" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="2" borderId="6" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2940,243 +2950,246 @@
     <xf numFmtId="170" fontId="0" fillId="2" borderId="3" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="8" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="31" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="35" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="25" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="33" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="25" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="25" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="24" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="24" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="2" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="24" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="8" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="31" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="35" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="25" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="33" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="24" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="25" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="25" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="24" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="24" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="24" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="2" borderId="4" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="2" borderId="24" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="24" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -3207,7 +3220,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -3267,352 +3280,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-C7F3-4075-AF0B-47F14120D6A7}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="es-CL"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'1.1'!$A$4:$B$35</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="32"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="30">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="31">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2008</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2009</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>2010</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>2011</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>2012</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>2013</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>2014</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>2015</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'1.1'!$C$4:$C$35</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
-                <c:pt idx="0">
-                  <c:v>930988</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>949145</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>960924</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>966741</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>988157</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1003511</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1024038</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1042444</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1042123</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1041683</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1037373</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1049336</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1026206</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1041077</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1063841</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1068151</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1076860</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1087318</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1087370</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1097139</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1115966</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1126388</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1135544</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1136701</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1147536</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1157390</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1163379</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1200825</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1188514</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1207023</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1216764</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1234072</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-EF1C-4F04-8CD0-D2DB9DE10874}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'1.1'!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Tendencia PIB</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-1.3888888888888867E-2"/>
-                  <c:y val="-8.7962962962962965E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -3801,6 +3473,350 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:f>'1.1'!$C$4:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>930988</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>949145</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>960924</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>966741</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>988157</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1003511</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1024038</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1042444</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1042123</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1041683</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1037373</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1049336</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1026206</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1041077</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1063841</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1068151</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1076860</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1087318</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1087370</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1097139</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1115966</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1126388</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1135544</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1136701</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1147536</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1157390</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1163379</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1200825</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1188514</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1207023</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1216764</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1234072</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EF1C-4F04-8CD0-D2DB9DE10874}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1.1'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tendencia PIB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.3888888888888867E-2"/>
+                  <c:y val="-8.7962962962962965E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-AC65-471B-A188-5C9249C09DE6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-CL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'1.1'!$A$4:$B$35</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="32"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="30">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2008</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2009</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2010</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2011</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>2012</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>2013</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>2014</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>2015</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
               <c:f>'1.1'!$D$4:$D$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
@@ -3905,7 +3921,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-EF1C-4F04-8CD0-D2DB9DE10874}"/>
             </c:ext>
@@ -4183,7 +4199,7 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -4255,6 +4271,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-ECB9-4BC2-B512-C249D808C270}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4271,372 +4290,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-6F91-433F-B0F7-225471647FA9}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="es-CL"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'1.10'!$A$4:$B$35</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="32"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>ene-mar</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
-                    <c:v>abr-jun</c:v>
-                  </c:pt>
-                  <c:pt idx="30">
-                    <c:v>jul-sep</c:v>
-                  </c:pt>
-                  <c:pt idx="31">
-                    <c:v>oct-dic</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2008</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2009</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>2010</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>2011</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>2012</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>2013</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>2014</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>2015</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'1.10'!$C$4:$C$35</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="32"/>
-                <c:pt idx="0">
-                  <c:v>6705</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6412</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5350</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4113</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3985</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4583</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4839</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6005</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5465</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5740</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6464</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7219</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7075</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7480</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6746</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7203</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>6931</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6889</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6069</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7338</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6483</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>7012</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>6502</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>6739</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>6630</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>6887</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>6247</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>6459</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>5925</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>5585</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>5060</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>5211</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6F91-433F-B0F7-225471647FA9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'1.10'!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Exportaciones nacional</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="-2.3148148148148147E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="31"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-4.6296296296296294E-3"/>
-                  <c:y val="-6.0185185185185182E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4825,6 +4483,373 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:f>'1.10'!$C$4:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>6705</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6412</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5350</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4113</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3985</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4583</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4839</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5465</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5740</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6464</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7219</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7075</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7480</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6746</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7203</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6931</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6889</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6069</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7338</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6483</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7012</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6502</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6739</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6630</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6887</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6247</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6459</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5925</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5585</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5060</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5211</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6F91-433F-B0F7-225471647FA9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1.10'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Exportaciones nacional</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.3148148148148147E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-ECB9-4BC2-B512-C249D808C270}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="31"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.6296296296296294E-3"/>
+                  <c:y val="-6.0185185185185182E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-ECB9-4BC2-B512-C249D808C270}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-CL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'1.10'!$A$4:$B$35</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="32"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>ene-mar</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
+                    <c:v>abr-jun</c:v>
+                  </c:pt>
+                  <c:pt idx="30">
+                    <c:v>jul-sep</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>oct-dic</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2008</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2009</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2010</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2011</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>2012</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>2013</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>2014</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>2015</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
               <c:f>'1.10'!$D$4:$D$35</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
@@ -4929,7 +4954,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6F91-433F-B0F7-225471647FA9}"/>
             </c:ext>
@@ -5207,7 +5232,7 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -5300,7 +5325,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E219-4903-9369-9923C4CADD19}"/>
             </c:ext>
@@ -5379,7 +5404,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-E219-4903-9369-9923C4CADD19}"/>
             </c:ext>
@@ -5459,7 +5484,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-E219-4903-9369-9923C4CADD19}"/>
             </c:ext>
@@ -5664,7 +5689,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -5725,6 +5750,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-20FF-47DB-9DFA-7115141D0778}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5742,11 +5770,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-4D4A-41DA-B063-473E218C36A7}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5763,7 +5791,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
               </c:ext>
@@ -5980,7 +6008,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-4D4A-41DA-B063-473E218C36A7}"/>
             </c:ext>
@@ -6026,11 +6054,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-4D4A-41DA-B063-473E218C36A7}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -6046,7 +6074,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
               </c:ext>
@@ -6263,7 +6291,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-4D4A-41DA-B063-473E218C36A7}"/>
             </c:ext>
@@ -6464,7 +6492,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -6521,6 +6549,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-01E4-41E4-BA38-2DA5FA76DE3F}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -6540,6 +6571,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-01E4-41E4-BA38-2DA5FA76DE3F}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -6557,11 +6591,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-F799-4D45-8023-71906DCD1A01}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -6595,7 +6629,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -7075,7 +7109,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F799-4D45-8023-71906DCD1A01}"/>
             </c:ext>
@@ -7125,6 +7159,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-01E4-41E4-BA38-2DA5FA76DE3F}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -7144,6 +7181,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-01E4-41E4-BA38-2DA5FA76DE3F}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -7161,11 +7201,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-F799-4D45-8023-71906DCD1A01}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -7199,7 +7239,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -7679,7 +7719,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-F799-4D45-8023-71906DCD1A01}"/>
             </c:ext>
@@ -7956,7 +7996,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -8020,11 +8060,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-4BB4-4C09-9B1C-74ACCD587F01}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8042,11 +8082,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-4BB4-4C09-9B1C-74ACCD587F01}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8064,11 +8104,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-1D6C-45B4-8D3A-C8446736DB81}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8086,11 +8126,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-4BB4-4C09-9B1C-74ACCD587F01}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8108,11 +8148,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-4BB4-4C09-9B1C-74ACCD587F01}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8130,11 +8170,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-4BB4-4C09-9B1C-74ACCD587F01}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8152,11 +8192,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-546C-490C-8E61-E19246E19C70}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8174,11 +8214,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-A66B-4897-82B0-8A4105D49D08}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8196,11 +8236,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-1D6C-45B4-8D3A-C8446736DB81}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8218,11 +8258,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-4BB4-4C09-9B1C-74ACCD587F01}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8240,11 +8280,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-546C-490C-8E61-E19246E19C70}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8262,11 +8302,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-4BB4-4C09-9B1C-74ACCD587F01}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8284,11 +8324,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-A66B-4897-82B0-8A4105D49D08}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -8325,7 +8365,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -8446,7 +8486,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-546C-490C-8E61-E19246E19C70}"/>
             </c:ext>
@@ -8492,11 +8532,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-546C-490C-8E61-E19246E19C70}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8514,11 +8554,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-A66B-4897-82B0-8A4105D49D08}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8536,11 +8576,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-A66B-4897-82B0-8A4105D49D08}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8558,11 +8598,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-A66B-4897-82B0-8A4105D49D08}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8580,11 +8620,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-A66B-4897-82B0-8A4105D49D08}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8602,11 +8642,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-4BB4-4C09-9B1C-74ACCD587F01}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8624,11 +8664,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-1D6C-45B4-8D3A-C8446736DB81}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8646,11 +8686,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-1D6C-45B4-8D3A-C8446736DB81}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8668,11 +8708,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-A66B-4897-82B0-8A4105D49D08}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8690,11 +8730,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-A66B-4897-82B0-8A4105D49D08}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8712,11 +8752,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-A66B-4897-82B0-8A4105D49D08}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -8734,11 +8774,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-4BB4-4C09-9B1C-74ACCD587F01}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -8775,7 +8815,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -8896,7 +8936,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-546C-490C-8E61-E19246E19C70}"/>
             </c:ext>
@@ -9079,7 +9119,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -9157,7 +9197,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -9284,7 +9324,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-CDBA-4733-8F40-157E6E04C41A}"/>
             </c:ext>
@@ -9348,7 +9388,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -9475,7 +9515,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-CDBA-4733-8F40-157E6E04C41A}"/>
             </c:ext>
@@ -9629,7 +9669,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -9690,11 +9730,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-0941-4DB5-AFC2-9F89D448D28B}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -9728,7 +9768,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -9855,7 +9895,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8CDB-42F3-95D3-4D77344A87C1}"/>
             </c:ext>
@@ -9919,7 +9959,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -10046,7 +10086,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8CDB-42F3-95D3-4D77344A87C1}"/>
             </c:ext>
@@ -10200,7 +10240,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -10263,6 +10303,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-F34D-4BB8-AA23-8586C0F0FC60}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -10274,11 +10317,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-FF8E-4BC1-BBDE-B4C7DB2E9B33}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -10312,7 +10355,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -10798,7 +10841,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FF8E-4BC1-BBDE-B4C7DB2E9B33}"/>
             </c:ext>
@@ -10864,6 +10907,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-F34D-4BB8-AA23-8586C0F0FC60}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -10881,11 +10927,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-FF8E-4BC1-BBDE-B4C7DB2E9B33}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -10919,7 +10965,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -11405,7 +11451,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-FF8E-4BC1-BBDE-B4C7DB2E9B33}"/>
             </c:ext>
@@ -11798,7 +11844,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -11861,6 +11907,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-6D31-476C-83EC-8D80978B0702}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -11880,6 +11929,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-6D31-476C-83EC-8D80978B0702}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -11897,11 +11949,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-1B29-4021-9722-81A68F07E856}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -11913,11 +11965,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-1B29-4021-9722-81A68F07E856}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -11951,7 +12003,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -12356,7 +12408,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-1B29-4021-9722-81A68F07E856}"/>
             </c:ext>
@@ -12422,6 +12474,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-6D31-476C-83EC-8D80978B0702}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -12441,6 +12496,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-6D31-476C-83EC-8D80978B0702}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -12452,11 +12510,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-1B29-4021-9722-81A68F07E856}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -12468,11 +12526,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-1B29-4021-9722-81A68F07E856}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -12506,7 +12564,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -12911,7 +12969,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-1B29-4021-9722-81A68F07E856}"/>
             </c:ext>
@@ -13329,7 +13387,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-1B29-4021-9722-81A68F07E856}"/>
             </c:ext>
@@ -13640,7 +13698,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -13706,6 +13764,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-C1EB-4D6B-BCFF-7F7392F05B29}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -13718,6 +13779,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-C1EB-4D6B-BCFF-7F7392F05B29}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -14232,7 +14296,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B50F-4186-8AED-015C5530EA29}"/>
             </c:ext>
@@ -14275,6 +14339,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-C1EB-4D6B-BCFF-7F7392F05B29}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -14287,6 +14354,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-C1EB-4D6B-BCFF-7F7392F05B29}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -14801,6 +14871,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-C1EB-4D6B-BCFF-7F7392F05B29}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -14845,6 +14920,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-C1EB-4D6B-BCFF-7F7392F05B29}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -14863,6 +14941,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-C1EB-4D6B-BCFF-7F7392F05B29}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -15377,6 +15458,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-C1EB-4D6B-BCFF-7F7392F05B29}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -15421,6 +15507,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-C1EB-4D6B-BCFF-7F7392F05B29}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -15439,6 +15528,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-C1EB-4D6B-BCFF-7F7392F05B29}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -15953,6 +16045,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-C1EB-4D6B-BCFF-7F7392F05B29}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -27009,43 +27106,43 @@
       <c r="I2" s="50"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="351" t="s">
+      <c r="A3" s="349" t="s">
         <v>401</v>
       </c>
-      <c r="B3" s="349" t="s">
+      <c r="B3" s="352" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="349"/>
-      <c r="D3" s="349"/>
-      <c r="E3" s="349"/>
-      <c r="F3" s="349" t="s">
+      <c r="C3" s="352"/>
+      <c r="D3" s="352"/>
+      <c r="E3" s="352"/>
+      <c r="F3" s="352" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="349"/>
-      <c r="H3" s="349"/>
-      <c r="I3" s="349"/>
+      <c r="G3" s="352"/>
+      <c r="H3" s="352"/>
+      <c r="I3" s="352"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="352"/>
-      <c r="B4" s="350" t="s">
+      <c r="A4" s="350"/>
+      <c r="B4" s="353" t="s">
         <v>298</v>
       </c>
-      <c r="C4" s="350"/>
-      <c r="D4" s="350" t="s">
+      <c r="C4" s="353"/>
+      <c r="D4" s="353" t="s">
         <v>329</v>
       </c>
-      <c r="E4" s="350"/>
-      <c r="F4" s="350" t="s">
+      <c r="E4" s="353"/>
+      <c r="F4" s="353" t="s">
         <v>298</v>
       </c>
-      <c r="G4" s="350"/>
-      <c r="H4" s="350" t="s">
+      <c r="G4" s="353"/>
+      <c r="H4" s="353" t="s">
         <v>329</v>
       </c>
-      <c r="I4" s="350"/>
+      <c r="I4" s="353"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="353"/>
+      <c r="A5" s="351"/>
       <c r="B5" s="86" t="s">
         <v>397</v>
       </c>
@@ -27321,45 +27418,45 @@
       <c r="J2" s="314"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="351" t="s">
+      <c r="A3" s="349" t="s">
         <v>401</v>
       </c>
-      <c r="B3" s="349" t="s">
+      <c r="B3" s="352" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="349"/>
-      <c r="D3" s="349"/>
-      <c r="E3" s="349"/>
-      <c r="F3" s="349" t="s">
+      <c r="C3" s="352"/>
+      <c r="D3" s="352"/>
+      <c r="E3" s="352"/>
+      <c r="F3" s="352" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="349"/>
-      <c r="H3" s="349"/>
-      <c r="I3" s="349"/>
+      <c r="G3" s="352"/>
+      <c r="H3" s="352"/>
+      <c r="I3" s="352"/>
       <c r="J3" s="195"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="352"/>
-      <c r="B4" s="350" t="s">
+      <c r="A4" s="350"/>
+      <c r="B4" s="353" t="s">
         <v>298</v>
       </c>
-      <c r="C4" s="350"/>
-      <c r="D4" s="350" t="s">
+      <c r="C4" s="353"/>
+      <c r="D4" s="353" t="s">
         <v>329</v>
       </c>
-      <c r="E4" s="350"/>
-      <c r="F4" s="350" t="s">
+      <c r="E4" s="353"/>
+      <c r="F4" s="353" t="s">
         <v>298</v>
       </c>
-      <c r="G4" s="350"/>
-      <c r="H4" s="350" t="s">
+      <c r="G4" s="353"/>
+      <c r="H4" s="353" t="s">
         <v>329</v>
       </c>
-      <c r="I4" s="350"/>
+      <c r="I4" s="353"/>
       <c r="J4" s="195"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="353"/>
+      <c r="A5" s="351"/>
       <c r="B5" s="86" t="s">
         <v>397</v>
       </c>
@@ -28344,7 +28441,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28873,7 +28970,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29117,8 +29214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29504,7 +29601,9 @@
       <c r="E22" s="262" t="s">
         <v>198</v>
       </c>
-      <c r="F22" s="257"/>
+      <c r="F22" s="399" t="s">
+        <v>426</v>
+      </c>
       <c r="G22" s="257"/>
       <c r="H22" s="257"/>
       <c r="I22" s="257"/>
@@ -30971,7 +31070,7 @@
         <v>13.558567047119141</v>
       </c>
       <c r="C5" s="12">
-        <v>11.851516723632812</v>
+        <v>11.851516723632813</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -33501,20 +33600,20 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="351" t="s">
+      <c r="A3" s="349" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="349" t="s">
+      <c r="B3" s="352" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="349"/>
-      <c r="D3" s="349" t="s">
+      <c r="C3" s="352"/>
+      <c r="D3" s="352" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="349"/>
+      <c r="E3" s="352"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="353"/>
+      <c r="A4" s="351"/>
       <c r="B4" s="86">
         <v>2010</v>
       </c>
@@ -35704,7 +35803,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>43.162033081054687</v>
+        <v>43.162033081054688</v>
       </c>
       <c r="B2">
         <v>10.663600921630859</v>
@@ -35721,7 +35820,7 @@
         <v>43.212192535400391</v>
       </c>
       <c r="B3">
-        <v>11.851516723632812</v>
+        <v>11.851516723632813</v>
       </c>
       <c r="C3">
         <v>59.183235168457031</v>
@@ -35736,7 +35835,7 @@
         <v>(mean) edad</v>
       </c>
       <c r="B5">
-        <v>43.162033081054687</v>
+        <v>43.162033081054688</v>
       </c>
       <c r="C5">
         <v>43.212192535400391</v>
@@ -35750,7 +35849,7 @@
         <v>10.663600921630859</v>
       </c>
       <c r="C6">
-        <v>11.851516723632812</v>
+        <v>11.851516723632813</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -35826,7 +35925,7 @@
         <v>43.212192535400391</v>
       </c>
       <c r="B3">
-        <v>11.851516723632812</v>
+        <v>11.851516723632813</v>
       </c>
       <c r="C3">
         <v>59.183235168457031</v>
@@ -35849,7 +35948,7 @@
         <v>13.558567047119141</v>
       </c>
       <c r="B6">
-        <v>11.851516723632812</v>
+        <v>11.851516723632813</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -36516,7 +36615,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
-        <v>185.75167846679687</v>
+        <v>185.75167846679688</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -36905,7 +37004,7 @@
         <v>48.159530639648438</v>
       </c>
       <c r="D7">
-        <v>50.662826538085937</v>
+        <v>50.662826538085938</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -41026,15 +41125,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010063FB1B1D25CB0745A389690B2E2CDE7A" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="717befc8328f7bdf6318d82e9e4a8783">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9ed0e8e1-aabc-4adb-a3c5-52e6530bbe04" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5a3e0ec156252a05b79e2b1081ddaf85" ns2:_="">
     <xsd:import namespace="9ed0e8e1-aabc-4adb-a3c5-52e6530bbe04"/>
@@ -41182,6 +41272,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1B02A05-038E-43EB-BB87-BC2D44E0F4BD}">
   <ds:schemaRefs>
@@ -41199,14 +41298,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84E9B3FC-BC50-47F1-889E-FFC0E53B90F3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF39A78A-68AF-4FF2-9292-3FF7CB02F03A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41222,4 +41313,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84E9B3FC-BC50-47F1-889E-FFC0E53B90F3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>